<commit_message>
changed file name from upload to uploads and install some libraries
</commit_message>
<xml_diff>
--- a/generated_schedule_output.xlsx
+++ b/generated_schedule_output.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R1 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
+          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R7 (60)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
+          <t>Monday 16:00-17:25, Thursday 14:30-15:55 (Q)</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R3 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Monday 16:00-17:25, Thursday 14:30-15:55 (Q)</t>
+          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
+          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R5 (60)</t>
+          <t>R1 (60)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
+          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R3 (60)</t>
+          <t>R4 (60)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
+          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R6 (60)</t>
+          <t>R1 (60)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
+          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R6 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Monday 16:00-17:25, Thursday 14:30-15:55 (Q)</t>
+          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R7 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
+          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R6 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
+          <t>Tuesday 16:00-17:25, Friday 14:30-15:55 (S)</t>
         </is>
       </c>
     </row>
@@ -841,7 +841,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R2 (60)</t>
+          <t>R1 (60)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
+          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
+          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R2 (60)</t>
+          <t>R4 (60)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R7 (60)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
+          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R3 (60)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tuesday 12:00-12:55, Wednesday 12:00-12:55, Friday 12:00-12:55 (G)</t>
+          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
+          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
minor flask bug fixed
</commit_message>
<xml_diff>
--- a/generated_schedule_output.xlsx
+++ b/generated_schedule_output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R5 (60)</t>
+          <t>R3 (60)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
+          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R7 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Monday 16:00-17:25, Thursday 14:30-15:55 (Q)</t>
+          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R5 (60)</t>
+          <t>R7 (60)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
+          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R2 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
+          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R5 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
+          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R1 (60)</t>
+          <t>R6 (60)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
+          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R6 (60)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
+          <t>Tuesday 14:30-15:55, Friday 16:00-17:25 (R)</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R1 (60)</t>
+          <t>R2 (60)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
+          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R2 (60)</t>
+          <t>R3 (60)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
+          <t>Tuesday 11:00-11:55,  Wednesday 16:00-17:25, Thursday 12-12:55 (E)</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
+          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Monday 11:00-11:55, Wednesday 10:00-10:55, Thursday 9:00-9:55 (C)</t>
+          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R5 (60)</t>
+          <t>R7 (60)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R1 (60)</t>
+          <t>R3 (60)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
+          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R5 (60)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R7 (60)</t>
+          <t>R1 (60)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
+          <t>Monday 9:00-9:55, Wednesday 11:00-11:55, Thursday 10:00-10:55 (A)</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R3 (60)</t>
+          <t>R6 (60)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tuesday 10:00-10:55, Thursday 11:00-11:55, Friday 10:00-10:55 (F)</t>
+          <t>Monday 10:00-10:55, Wednesday 9:00-9:55, Friday 9:00-9:55 (B)</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R4 (60)</t>
+          <t>R7 (60)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Monday 12:00-12:55, Tuesday 9:00-9:55, Friday 11:00-11:55 (D)</t>
+          <t>Monday 14:30-15:55, Thursday 16:00-17:25 (P)</t>
         </is>
       </c>
     </row>

</xml_diff>